<commit_message>
- fixed the use of OTC in Nexial
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/data/webasync-showcase.data.xlsx
+++ b/src/test/resources/showcase/artifact/data/webasync-showcase.data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB3A124-6F5E-1449-829A-0670B901978B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1E9810-BC0A-984E-B022-0845A42EF3BB}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7360" yWindow="440" windowWidth="33600" windowHeight="20540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="-21160" windowWidth="38400" windowHeight="7040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
     <definedName name="webcookie">'[1]#system'!$O$2:$O$8</definedName>
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>true</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>nexial.inspectOnPause</t>
+  </si>
+  <si>
+    <t>10000</t>
   </si>
 </sst>
 </file>
@@ -583,7 +586,7 @@
   <dimension ref="A1:AAA10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -680,6 +683,9 @@
         <v>13</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="HA9" s="4"/>
@@ -708,7 +714,7 @@
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
+  <conditionalFormatting sqref="B1:B8 B10:B1048576 C9">
     <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>

</xml_diff>